<commit_message>
Fix some mapping issues in io-model/ItICM (#50)
</commit_message>
<xml_diff>
--- a/InputData/io-model/ItICM/Industry to ISIC Code Map.xlsx
+++ b/InputData/io-model/ItICM/Industry to ISIC Code Map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\add-outputs\ItICM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\io-model\ItICM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D27857-4F77-467C-89F0-3816B420CD8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB97F830-B4B5-4069-8ACE-BCC0DE0A0E01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2850" yWindow="375" windowWidth="24765" windowHeight="17010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -1028,13 +1028,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1085,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="V3">
-        <v>0.25</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="W3">
         <v>0</v>
@@ -1367,13 +1367,13 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.75</v>
+        <v>0.1</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -1537,7 +1537,7 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <v>0.75</v>
+        <v>0.33300000000000002</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -1712,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1763,7 +1763,7 @@
         <v>1</v>
       </c>
       <c r="V9">
-        <v>0</v>
+        <v>0.33400000000000002</v>
       </c>
       <c r="W9">
         <v>0</v>

</xml_diff>